<commit_message>
add batch at import saldo awal coa
</commit_message>
<xml_diff>
--- a/public/template-excel/template-saldo-awal.xlsx
+++ b/public/template-excel/template-saldo-awal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\simpin\public\template-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\simpin\public\template-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F249E6F8-DC57-4D9B-A190-04253CE63A0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890A943F-6D16-4DE1-9CA5-99131A1EB1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>100.00.000</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>besar_saldo_awal</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>13-02-2020</t>
   </si>
 </sst>
 </file>
@@ -869,32 +875,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>